<commit_message>
ported to kicad 7.0 from old project
</commit_message>
<xml_diff>
--- a/hdw/Incrementor/Incrementor.xlsx
+++ b/hdw/Incrementor/Incrementor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Incrementor\hdw\Incrementor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF2E38C-360D-4705-999E-88AF7EBED495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B37605-B5C9-4FA4-9178-35190D7137AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="135">
-  <si>
-    <t>Item</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
   <si>
     <t>Qty</t>
   </si>
@@ -112,9 +109,6 @@
     <t>CDSOD323-T03SCT-ND</t>
   </si>
   <si>
-    <t>3mm</t>
-  </si>
-  <si>
     <t>J201</t>
   </si>
   <si>
@@ -250,9 +244,6 @@
     <t>CAT16-102J8LFCT-ND</t>
   </si>
   <si>
-    <t>Cap_Touch</t>
-  </si>
-  <si>
     <t>U201</t>
   </si>
   <si>
@@ -352,6 +343,12 @@
     <t>X401</t>
   </si>
   <si>
+    <t>ECS-327KE</t>
+  </si>
+  <si>
+    <t>XC1751CT-ND</t>
+  </si>
+  <si>
     <t>C201, C303, C401, C404, C407, C501, C502, C503, C504, C505, C506, C507, C508, C601, C602, C603, C604, C605, C606, C607, C608, C609, C702, C703, C704, C707, C708, C709, C712, C713, C715, C717, C801, C901, C1001, C1101, C1201, C1301, C1401, C1501, C1601, C1701, C1801, C1901</t>
   </si>
   <si>
@@ -373,9 +370,6 @@
     <t>D801, D1901</t>
   </si>
   <si>
-    <t>H2001, H2002, H2003, H2004</t>
-  </si>
-  <si>
     <t>MK2001, MK2002, MK2003, MK2004</t>
   </si>
   <si>
@@ -397,9 +391,6 @@
     <t>RN901, RN1001, RN1101, RN1201, RN1301, RN1401, RN1501, RN1601, RN1701, RN1801</t>
   </si>
   <si>
-    <t>SW701, SW702, SW703</t>
-  </si>
-  <si>
     <t>U501, U502, U503, U504, U505, U506</t>
   </si>
   <si>
@@ -421,17 +412,26 @@
     <t>U902, U1002, U1102, U1202, U1302, U1402, U1502, U1602, U1702, U1802</t>
   </si>
   <si>
-    <t>XC1751CT-ND</t>
-  </si>
-  <si>
-    <t>ECS-327KE</t>
+    <t>RMCF0603FT51K1CT-ND</t>
+  </si>
+  <si>
+    <t>311-1.15KHRCT-ND</t>
+  </si>
+  <si>
+    <t>749-1665-1-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT6K04CT-ND</t>
+  </si>
+  <si>
+    <t>311-16.5KHRCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +562,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -916,7 +923,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1274,27 +1281,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="24.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="15.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1302,64 +1309,52 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:4" ht="319" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="B2" s="1">
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
+    </row>
+    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="B3" s="1">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>3</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1370,14 +1365,10 @@
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1388,47 +1379,38 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>6</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>7</v>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1439,13 +1421,10 @@
       <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -1456,699 +1435,541 @@
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>10</v>
+    </row>
+    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="B11" s="1">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>11</v>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
       <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="1">
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>39</v>
+      <c r="C17" s="2">
+        <v>14702</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>17</v>
+    </row>
+    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2">
+        <v>14702</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="2">
-        <v>14702</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" s="2">
-        <v>14702</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B23" s="1">
         <v>50</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
       <c r="B24" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
       <c r="B31" s="1">
-        <v>9</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>121</v>
+        <v>3</v>
+      </c>
+      <c r="C31" s="1">
+        <v>499</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1">
+        <v>100</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1">
+    </row>
+    <row r="33" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="1">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="1">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4072</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4017</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="1">
+        <v>9</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="1">
         <v>3</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" s="1">
-        <v>499</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="C42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="1">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1">
+    </row>
+    <row r="45" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="1">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="1">
         <v>10</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1">
-        <v>3</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1">
-        <v>6</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="1">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="1">
-        <v>4072</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="1">
-        <v>4017</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1">
-        <v>9</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1">
-        <v>3</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1">
-        <v>3</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1">
+        <v>4026</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
       <c r="B47" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E47" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
-        <v>47</v>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="B48" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D48" s="1">
-        <v>4026</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" s="1">
-        <v>10</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D49" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>